<commit_message>
new folders for testing (delete later)
</commit_message>
<xml_diff>
--- a/src/main/resources/cardiac_diseases/test.drl.xlsx
+++ b/src/main/resources/cardiac_diseases/test.drl.xlsx
@@ -8,24 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS\Cardiac_diseases\src\main\resources\cardiac_diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2019589B-76A7-4491-AC5E-3B875E9DFA75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4EAB62-3FA2-4EF8-983B-D289F842FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>RuleSet</t>
   </si>
@@ -45,53 +56,72 @@
     <t>RuleTable testPatient</t>
   </si>
   <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>cardiac_diseases.Patient, cardiac_diseases.Symptom, cardiac_diseases.Disease</t>
+  </si>
+  <si>
+    <t>symptom</t>
+  </si>
+  <si>
+    <t>$patient:Patient</t>
+  </si>
+  <si>
+    <t>NAME</t>
+  </si>
+  <si>
     <t>Unit</t>
   </si>
   <si>
     <t>PatientUnit</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>cardiac_diseases.Patient, cardiac_diseases.Symptom, cardiac_diseases.Disease</t>
-  </si>
-  <si>
-    <t>symptom</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>$patient:Patient</t>
-  </si>
-  <si>
-    <t>"whatever"</t>
-  </si>
-  <si>
-    <t>$patient.setAge($param2);</t>
-  </si>
-  <si>
-    <t>System.out.println("hello"+$param);</t>
-  </si>
-  <si>
-    <t>age</t>
-  </si>
-  <si>
-    <t>NAME</t>
-  </si>
-  <si>
-    <t>test3</t>
-  </si>
-  <si>
-    <t>test4</t>
+    <t>EscapeQuotes</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>age == 20</t>
+  </si>
+  <si>
+    <t>$param</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">modify($patient){
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="30"/>
+        <rFont val="メイリオ"/>
+      </rPr>
+      <t xml:space="preserve"> setAge($1),
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="30"/>
+        <rFont val="メイリオ"/>
+        <charset val="128"/>
+      </rPr>
+      <t xml:space="preserve"> setName($2);
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>30, "other"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -120,6 +150,21 @@
       <name val="メイリオ"/>
       <charset val="128"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="メイリオ"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="30"/>
+      <name val="メイリオ"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="30"/>
+      <name val="メイリオ"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -147,7 +192,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -207,6 +252,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -215,7 +299,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -246,6 +330,21 @@
     <xf numFmtId="49" fontId="4" fillId="2" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="4" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="3" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,166 +627,126 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D7" sqref="D7:D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="16.6640625" customWidth="1"/>
-    <col min="3" max="3" width="23.33203125" customWidth="1"/>
-    <col min="4" max="4" width="35.6640625" customWidth="1"/>
-    <col min="5" max="5" width="30.77734375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.44140625" customWidth="1"/>
+    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" ht="16.2">
-      <c r="B2" s="3"/>
+    <row r="1" spans="1:4" ht="16.2">
+      <c r="A1" s="3"/>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" ht="16.2">
+      <c r="A2" s="3"/>
+      <c r="B2" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="C2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="2:5" ht="16.2">
-      <c r="B3" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="16.2">
+      <c r="A3" s="3"/>
+      <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="C3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="4"/>
-    </row>
-    <row r="4" spans="2:5" ht="16.2">
-      <c r="B4" s="3"/>
-      <c r="C4" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="4"/>
-    </row>
-    <row r="5" spans="2:5">
-      <c r="B5" s="3"/>
+        <v>12</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" ht="16.2">
+      <c r="A4" s="3"/>
+      <c r="B4" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-    </row>
-    <row r="6" spans="2:5" ht="16.2">
-      <c r="B6" s="3"/>
-      <c r="C6" s="11" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="16.2">
+      <c r="A6" s="3"/>
+      <c r="B6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="D6" s="12"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="2:5" ht="16.2">
+      <c r="C6" s="12"/>
+      <c r="D6" s="13"/>
+    </row>
+    <row r="7" spans="1:4" ht="16.2">
+      <c r="A7" s="6" t="s">
+        <v>10</v>
+      </c>
       <c r="B7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" ht="16.2">
+      <c r="A8" s="3"/>
+      <c r="B8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+    </row>
+    <row r="9" spans="1:4" ht="64.8">
+      <c r="A9" s="7"/>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" ht="16.2">
-      <c r="B8" s="3"/>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-    </row>
-    <row r="9" spans="2:5" ht="16.2">
-      <c r="B9" s="7"/>
-      <c r="C9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="18"/>
+    </row>
+    <row r="10" spans="1:4" ht="16.2">
+      <c r="A10" s="3"/>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" ht="16.2">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="2:5" ht="16.2">
-      <c r="B10" s="3"/>
-      <c r="C10" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="16.2">
-      <c r="B11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="2">
-        <v>20</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="2:5" ht="16.2">
-      <c r="B12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C12" s="2">
-        <v>20</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" ht="16.2">
-      <c r="B13" s="1" t="s">
+      <c r="C11" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="C13" s="2">
-        <v>20</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" ht="16.2">
-      <c r="B14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="2">
-        <v>20</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E14" s="2">
-        <v>2</v>
-      </c>
+      <c r="D11" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
managed exceptions in hospitalMenu
</commit_message>
<xml_diff>
--- a/src/main/resources/cardiac_diseases/test.drl.xlsx
+++ b/src/main/resources/cardiac_diseases/test.drl.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DSS\Cardiac_diseases\src\main\resources\cardiac_diseases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA4EAB62-3FA2-4EF8-983B-D289F842FD8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{231EC6D4-E068-4133-BC62-12A4C24D3A68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>symptom</t>
   </si>
   <si>
-    <t>$patient:Patient</t>
-  </si>
-  <si>
     <t>NAME</t>
   </si>
   <si>
@@ -87,6 +84,9 @@
   </si>
   <si>
     <t>$param</t>
+  </si>
+  <si>
+    <t>30, "other"</t>
   </si>
   <si>
     <r>
@@ -114,7 +114,7 @@
     </r>
   </si>
   <si>
-    <t>30, "other"</t>
+    <t>$patient: Patient</t>
   </si>
 </sst>
 </file>
@@ -630,7 +630,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7:D11"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -665,20 +665,20 @@
     <row r="3" spans="1:4" ht="16.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>11</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>12</v>
       </c>
       <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="16.2">
       <c r="A4" s="3"/>
       <c r="B4" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="15" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="15" t="s">
-        <v>14</v>
       </c>
       <c r="D4" s="4"/>
     </row>
@@ -698,7 +698,7 @@
     </row>
     <row r="7" spans="1:4" ht="16.2">
       <c r="A7" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>2</v>
@@ -711,7 +711,7 @@
     <row r="8" spans="1:4" ht="16.2">
       <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="8"/>
@@ -719,7 +719,7 @@
     <row r="9" spans="1:4" ht="64.8">
       <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="17" t="s">
         <v>17</v>
@@ -741,10 +741,10 @@
         <v>6</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2"/>
     </row>

</xml_diff>